<commit_message>
table pos A for OASIS added
</commit_message>
<xml_diff>
--- a/results/Paper/table2_LogReg nice.xlsx
+++ b/results/Paper/table2_LogReg nice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D646470C-5C74-7346-AB23-2098E72D5AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376CA000-0AE8-7B47-8C62-4ADF70508124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
@@ -100,20 +100,20 @@
     <t>7 - 10 / 46 - 51</t>
   </si>
   <si>
-    <t>4 - 6  / 38 - 45</t>
-  </si>
-  <si>
     <t>0 - 3 / 0 - 37</t>
   </si>
   <si>
     <t>&gt; 10 / &gt; 51</t>
+  </si>
+  <si>
+    <t>4 - 6 / 38 - 45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -130,14 +130,20 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -149,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -172,38 +178,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,21 +637,21 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -926,13 +1013,13 @@
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>1.0144956199999999</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>0.86591132000000004</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>1.18904553</v>
       </c>
     </row>
@@ -996,13 +1083,13 @@
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>0.97231027999999997</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>0.82639618999999997</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>1.1475238800000001</v>
       </c>
     </row>
@@ -1024,13 +1111,13 @@
       <c r="A28" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>1.14023561</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>1.08933857</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>1.1935783099999999</v>
       </c>
     </row>
@@ -1038,13 +1125,13 @@
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>1.26278136</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>1.1699924399999999</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>1.3633466000000001</v>
       </c>
     </row>
@@ -1052,13 +1139,13 @@
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>1.1659218099999999</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>1.0704266899999999</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="5">
         <v>1.2700923799999999</v>
       </c>
     </row>
@@ -1105,216 +1192,216 @@
   <dimension ref="B2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="10"/>
-    <col min="4" max="4" width="16.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="10"/>
+    <col min="1" max="1" width="3.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="6"/>
+    <col min="4" max="4" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="11" t="str">
+      <c r="D4" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B2, 2), " (", ROUND(MIMIC!C2,2), " - ", ROUND(MIMIC!D2,2),  ")")</f>
         <v>1.08 (1.03 - 1.13)</v>
       </c>
-      <c r="E4" s="11" t="str">
+      <c r="E4" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B3, 2), " (", ROUND(MIMIC!C3,2), " - ", ROUND(MIMIC!D3,2),  ")")</f>
         <v>1.02 (0.93 - 1.11)</v>
       </c>
-      <c r="F4" s="11" t="str">
+      <c r="F4" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B4, 2), " (", ROUND(MIMIC!C4,2), " - ", ROUND(MIMIC!D4,2),  ")")</f>
         <v>0.92 (0.74 - 1.14)</v>
       </c>
-      <c r="G4" s="11" t="str">
+      <c r="G4" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B5, 2), " (", ROUND(MIMIC!C5,2), " - ", ROUND(MIMIC!D5,2),  ")")</f>
         <v>1.1 (1.02 - 1.19)</v>
       </c>
-      <c r="H4" s="11" t="str">
+      <c r="H4" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B6, 2), " (", ROUND(MIMIC!C6,2), " - ", ROUND(MIMIC!D6,2),  ")")</f>
         <v>1.16 (1.05 - 1.28)</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="str">
+      <c r="D5" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B18, 2), " (", ROUND(MIMIC!C18,2), " - ", ROUND(MIMIC!D18,2),  ")")</f>
         <v>1.08 (1.02 - 1.13)</v>
       </c>
-      <c r="E5" s="11" t="str">
+      <c r="E5" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B19, 2), " (", ROUND(MIMIC!C19,2), " - ", ROUND(MIMIC!D19,2),  ")")</f>
         <v>1.04 (0.95 - 1.13)</v>
       </c>
-      <c r="F5" s="11" t="str">
+      <c r="F5" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B20, 2), " (", ROUND(MIMIC!C20,2), " - ", ROUND(MIMIC!D20,2),  ")")</f>
         <v>1 (0.92 - 1.1)</v>
       </c>
-      <c r="G5" s="11" t="str">
+      <c r="G5" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B21, 2), " (", ROUND(MIMIC!C21,2), " - ", ROUND(MIMIC!D21,2),  ")")</f>
         <v>1.01 (0.87 - 1.19)</v>
       </c>
-      <c r="H5" s="11" t="str">
+      <c r="H5" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B22, 2), " (", ROUND(MIMIC!C22,2), " - ", ROUND(MIMIC!D22,2),  ")")</f>
         <v>1.18 (1.02 - 1.38)</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="11" t="str">
+      <c r="D6" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B7, 2), " (", ROUND(MIMIC!C7,2), " - ", ROUND(MIMIC!D7,2),  ")")</f>
         <v>0.84 (0.78 - 0.91)</v>
       </c>
-      <c r="E6" s="11" t="str">
+      <c r="E6" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B8, 2), " (", ROUND(MIMIC!C8,2), " - ", ROUND(MIMIC!D8,2),  ")")</f>
         <v>0.88 (0.68 - 1.15)</v>
       </c>
-      <c r="F6" s="11" t="str">
+      <c r="F6" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B9, 2), " (", ROUND(MIMIC!C9,2), " - ", ROUND(MIMIC!D9,2),  ")")</f>
         <v>1.07 (0.91 - 1.26)</v>
       </c>
-      <c r="G6" s="11" t="str">
+      <c r="G6" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B10, 2), " (", ROUND(MIMIC!C10,2), " - ", ROUND(MIMIC!D10,2),  ")")</f>
         <v>0.77 (0.67 - 0.89)</v>
       </c>
-      <c r="H6" s="11" t="str">
+      <c r="H6" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B11, 2), " (", ROUND(MIMIC!C11,2), " - ", ROUND(MIMIC!D11,2),  ")")</f>
         <v>0.79 (0.7 - 0.91)</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="9"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="11" t="str">
+      <c r="D7" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B23, 2), " (", ROUND(MIMIC!C23,2), " - ", ROUND(MIMIC!D23,2),  ")")</f>
         <v>0.8 (0.74 - 0.86)</v>
       </c>
-      <c r="E7" s="11" t="str">
+      <c r="E7" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B24, 2), " (", ROUND(MIMIC!C24,2), " - ", ROUND(MIMIC!D24,2),  ")")</f>
         <v>0.68 (0.59 - 0.78)</v>
       </c>
-      <c r="F7" s="11" t="str">
+      <c r="F7" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B25, 2), " (", ROUND(MIMIC!C25,2), " - ", ROUND(MIMIC!D25,2),  ")")</f>
         <v>0.79 (0.69 - 0.91)</v>
       </c>
-      <c r="G7" s="11" t="str">
+      <c r="G7" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B26, 2), " (", ROUND(MIMIC!C26,2), " - ", ROUND(MIMIC!D26,2),  ")")</f>
         <v>0.97 (0.83 - 1.15)</v>
       </c>
-      <c r="H7" s="11" t="str">
+      <c r="H7" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B27, 2), " (", ROUND(MIMIC!C27,2), " - ", ROUND(MIMIC!D27,2),  ")")</f>
         <v>0.91 (0.75 - 1.11)</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="str">
+      <c r="D8" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B12, 2), " (", ROUND(MIMIC!C12,2), " - ", ROUND(MIMIC!D12,2),  ")")</f>
         <v>1.21 (1.15 - 1.27)</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B13, 2), " (", ROUND(MIMIC!C13,2), " - ", ROUND(MIMIC!D13,2),  ")")</f>
         <v>1.14 (1.04 - 1.24)</v>
       </c>
-      <c r="F8" s="11" t="str">
+      <c r="F8" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B14, 2), " (", ROUND(MIMIC!C14,2), " - ", ROUND(MIMIC!D14,2),  ")")</f>
         <v>1.12 (0.86 - 1.44)</v>
       </c>
-      <c r="G8" s="11" t="str">
+      <c r="G8" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B15, 2), " (", ROUND(MIMIC!C15,2), " - ", ROUND(MIMIC!D15,2),  ")")</f>
         <v>1.24 (1.15 - 1.34)</v>
       </c>
-      <c r="H8" s="11" t="str">
+      <c r="H8" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B16, 2), " (", ROUND(MIMIC!C16,2), " - ", ROUND(MIMIC!D16,2),  ")")</f>
         <v>1.27 (1.15 - 1.4)</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="D9" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B28, 2), " (", ROUND(MIMIC!C28,2), " - ", ROUND(MIMIC!D28,2),  ")")</f>
         <v>1.14 (1.09 - 1.19)</v>
       </c>
-      <c r="E9" s="11" t="str">
+      <c r="E9" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B29, 2), " (", ROUND(MIMIC!C29,2), " - ", ROUND(MIMIC!D29,2),  ")")</f>
         <v>1.26 (1.17 - 1.36)</v>
       </c>
-      <c r="F9" s="11" t="str">
+      <c r="F9" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B30, 2), " (", ROUND(MIMIC!C30,2), " - ", ROUND(MIMIC!D30,2),  ")")</f>
         <v>1.17 (1.07 - 1.27)</v>
       </c>
-      <c r="G9" s="11" t="str">
+      <c r="G9" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B31, 2), " (", ROUND(MIMIC!C31,2), " - ", ROUND(MIMIC!D31,2),  ")")</f>
         <v>0.93 (0.85 - 1.03)</v>
       </c>
-      <c r="H9" s="11" t="str">
+      <c r="H9" s="12" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!B32, 2), " (", ROUND(MIMIC!C32,2), " - ", ROUND(MIMIC!D32,2),  ")")</f>
         <v>1.01 (0.89 - 1.15)</v>
       </c>

</xml_diff>

<commit_message>
changes to log reg to homog. with TMLE
</commit_message>
<xml_diff>
--- a/results/Paper/table2_LogReg nice.xlsx
+++ b/results/Paper/table2_LogReg nice.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376CA000-0AE8-7B47-8C62-4ADF70508124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE72E92-F5A3-FF4F-B9D7-98C15C26F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15500" yWindow="740" windowWidth="19060" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="processed" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -155,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,24 +164,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -193,24 +176,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -219,22 +185,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -246,21 +197,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -269,28 +228,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="183" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -637,34 +581,34 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.0811203196108401</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.0304401047431799</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.13437449017014</v>
+      <c r="B2">
+        <v>1.08146703683185</v>
+      </c>
+      <c r="C2">
+        <v>1.0307351770261</v>
+      </c>
+      <c r="D2">
+        <v>1.13477728766938</v>
       </c>
       <c r="E2" s="1"/>
       <c r="H2" s="2"/>
@@ -679,18 +623,18 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>1.0166082878399201</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.93303260104284602</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.1084005378681701</v>
+      <c r="B3" s="4">
+        <v>1.01409555</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.93067527999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.10572118</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="2"/>
@@ -710,18 +654,18 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0.91882697300000005</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.73583220900000001</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.1405006360000001</v>
+        <v>0.91082368000000002</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.72952894000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.1303955400000001</v>
       </c>
       <c r="E4" s="1"/>
       <c r="G4" s="2"/>
@@ -745,14 +689,14 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>1.1035944796267401</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.02199154182262</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.19199912426818</v>
+      <c r="B5">
+        <v>1.1047718678115199</v>
+      </c>
+      <c r="C5">
+        <v>1.0229229392972099</v>
+      </c>
+      <c r="D5">
+        <v>1.1934565580798699</v>
       </c>
       <c r="E5" s="1"/>
       <c r="G5" s="2"/>
@@ -776,14 +720,14 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
-        <v>1.1573073380000001</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.0494563669999999</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.275894801</v>
+      <c r="B6">
+        <v>1.15826719222395</v>
+      </c>
+      <c r="C6">
+        <v>1.05039029259158</v>
+      </c>
+      <c r="D6">
+        <v>1.2768775054309001</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="2"/>
@@ -803,33 +747,33 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.84387668305804298</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.77900075757655796</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.91471466869565499</v>
+      <c r="B7" s="4">
+        <v>0.84829365000000001</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.78301156000000005</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.91958359000000001</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.88090088998946703</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.67876512103067399</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.15498496978098</v>
+      <c r="B8" s="4">
+        <v>0.89128492999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.68686272000000004</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.1684383</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -837,14 +781,14 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>1.06744196717327</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.90557215638011201</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.2606388241764901</v>
+      <c r="B9">
+        <v>1.06671501106769</v>
+      </c>
+      <c r="C9">
+        <v>0.90485768404126898</v>
+      </c>
+      <c r="D9">
+        <v>1.2599210932092699</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -852,14 +796,14 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.76949326161522402</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.66768214864471398</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.88854240913828797</v>
+      <c r="B10">
+        <v>0.77530355422302999</v>
+      </c>
+      <c r="C10">
+        <v>0.672597734935243</v>
+      </c>
+      <c r="D10">
+        <v>0.89542556094065695</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -867,29 +811,29 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.794560661703965</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.69613714697925799</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.90833594099691195</v>
+      <c r="B11">
+        <v>0.79851582214818995</v>
+      </c>
+      <c r="C11">
+        <v>0.69961261489658</v>
+      </c>
+      <c r="D11">
+        <v>0.91285788217013597</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>1.2088504498045201</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.15162038744722</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.26902835999122</v>
+      <c r="B12" s="4">
+        <v>1.2064978799999999</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.14945338</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.26647643</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -897,44 +841,44 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
-        <v>1.13976315015008</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.0446387841592999</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1.24450121806634</v>
+      <c r="B13">
+        <v>1.1414986742231199</v>
+      </c>
+      <c r="C13">
+        <v>1.0463322015207699</v>
+      </c>
+      <c r="D13">
+        <v>1.2462766358144599</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1">
-        <v>1.1167332498446101</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.85862064676684302</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1.4409736369896</v>
+      <c r="B14" s="4">
+        <v>1.11623666</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.85846268999999997</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.43991779</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1">
-        <v>1.2398451046843</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.1498798504661001</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.3372113919767901</v>
+      <c r="B15" s="4">
+        <v>1.2347035799999999</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.14524991</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.33150396</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -942,14 +886,14 @@
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1">
-        <v>1.2677502059638901</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.1493043307150701</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1.3979083079835399</v>
+      <c r="B16">
+        <v>1.26460824571479</v>
+      </c>
+      <c r="C16">
+        <v>1.14663569766725</v>
+      </c>
+      <c r="D16">
+        <v>1.3942213155537699</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -972,27 +916,27 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <v>1.07744399022185</v>
+        <v>1.0669894648498599</v>
       </c>
       <c r="C18">
-        <v>1.02450999489705</v>
+        <v>1.0137422304286099</v>
       </c>
       <c r="D18">
-        <v>1.1331776093946899</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.1230989678063501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19">
-        <v>1.0390443686583899</v>
-      </c>
-      <c r="C19">
-        <v>0.95214302627873104</v>
-      </c>
-      <c r="D19">
-        <v>1.1344576954564101</v>
+      <c r="B19" s="4">
+        <v>1.02011228</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.93399730000000003</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.11472412</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,27 +944,27 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>1.00414279433064</v>
+        <v>0.99408935087309602</v>
       </c>
       <c r="C20">
-        <v>0.91856546638327197</v>
+        <v>0.90823046977910304</v>
       </c>
       <c r="D20">
-        <v>1.0978323157348</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>1.0882020489382001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5">
-        <v>1.0144956199999999</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0.86591132000000004</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1.18904553</v>
+      <c r="B21">
+        <v>1.00363378721699</v>
+      </c>
+      <c r="C21">
+        <v>0.85326019977818202</v>
+      </c>
+      <c r="D21">
+        <v>1.1807748954742201</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,13 +972,13 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>1.18467870862929</v>
+        <v>1.1965954397215499</v>
       </c>
       <c r="C22">
-        <v>1.0173343024916901</v>
+        <v>1.02725553059355</v>
       </c>
       <c r="D22">
-        <v>1.3776921495976</v>
+        <v>1.3920086765041</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,13 +986,13 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>0.80013910739480498</v>
+        <v>0.80304021853969099</v>
       </c>
       <c r="C23">
-        <v>0.74075775708439195</v>
+        <v>0.74334843511148097</v>
       </c>
       <c r="D23">
-        <v>0.864817067176059</v>
+        <v>0.86806558680703305</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,13 +1000,13 @@
         <v>6</v>
       </c>
       <c r="B24">
-        <v>0.67936580590962803</v>
+        <v>0.68403221205276699</v>
       </c>
       <c r="C24">
-        <v>0.59128287265900803</v>
+        <v>0.59525088586999297</v>
       </c>
       <c r="D24">
-        <v>0.78189667696141196</v>
+        <v>0.78740734766391496</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,27 +1014,27 @@
         <v>7</v>
       </c>
       <c r="B25">
-        <v>0.790294545507502</v>
+        <v>0.79620818927738701</v>
       </c>
       <c r="C25">
-        <v>0.68576954921199296</v>
+        <v>0.69084194848076097</v>
       </c>
       <c r="D25">
-        <v>0.912638995873433</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>0.91955552614854597</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="5">
-        <v>0.97231027999999997</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0.82639618999999997</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1.1475238800000001</v>
+      <c r="B26">
+        <v>0.97240357184506898</v>
+      </c>
+      <c r="C26">
+        <v>0.82632269229098698</v>
+      </c>
+      <c r="D26">
+        <v>1.1478224316149299</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,55 +1042,55 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>0.90912707472086995</v>
+        <v>0.89922307020937997</v>
       </c>
       <c r="C27">
-        <v>0.74615868027565502</v>
+        <v>0.73734337763117297</v>
       </c>
       <c r="D27">
-        <v>1.1120680012089601</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>1.10086123539641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="5">
-        <v>1.14023561</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1.08933857</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1.1935783099999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>1.1389446949191699</v>
+      </c>
+      <c r="C28">
+        <v>1.0881409871118599</v>
+      </c>
+      <c r="D28">
+        <v>1.19218757966544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="5">
-        <v>1.26278136</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1.1699924399999999</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1.3633466000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>1.2627385470749799</v>
+      </c>
+      <c r="C29">
+        <v>1.1702301266987101</v>
+      </c>
+      <c r="D29">
+        <v>1.36297806880328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="5">
-        <v>1.1659218099999999</v>
-      </c>
-      <c r="C30" s="5">
-        <v>1.0704266899999999</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1.2700923799999999</v>
+      <c r="B30">
+        <v>1.16525883394225</v>
+      </c>
+      <c r="C30">
+        <v>1.0699031603158899</v>
+      </c>
+      <c r="D30">
+        <v>1.2692671831695801</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,13 +1098,13 @@
         <v>8</v>
       </c>
       <c r="B31">
-        <v>0.93498346080447203</v>
+        <v>0.93530196488079498</v>
       </c>
       <c r="C31">
-        <v>0.84537091775332196</v>
+        <v>0.84546248207960495</v>
       </c>
       <c r="D31">
-        <v>1.03423796670018</v>
+        <v>1.03483538710417</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1168,13 +1112,13 @@
         <v>9</v>
       </c>
       <c r="B32">
-        <v>1.01343604026168</v>
+        <v>1.01200864504824</v>
       </c>
       <c r="C32">
-        <v>0.89213864167997603</v>
+        <v>0.89027965981635404</v>
       </c>
       <c r="D32">
-        <v>1.15124456652797</v>
+        <v>1.15043617568598</v>
       </c>
     </row>
   </sheetData>
@@ -1191,218 +1135,218 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46007BA-F4A7-5F42-81F4-3F357B170096}">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="196" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="6"/>
-    <col min="4" max="4" width="16.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="3.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="5"/>
+    <col min="4" max="4" width="16.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B2, 2), " (", ROUND(MIMIC!C2,2), " - ", ROUND(MIMIC!D2,2),  ")")</f>
+      <c r="D4" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B2, 2), " (", ROUND(data!C2,2), " - ", ROUND(data!D2,2),  ")")</f>
         <v>1.08 (1.03 - 1.13)</v>
       </c>
-      <c r="E4" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B3, 2), " (", ROUND(MIMIC!C3,2), " - ", ROUND(MIMIC!D3,2),  ")")</f>
+      <c r="E4" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B3, 2), " (", ROUND(data!C3,2), " - ", ROUND(data!D3,2),  ")")</f>
+        <v>1.01 (0.93 - 1.11)</v>
+      </c>
+      <c r="F4" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B4, 2), " (", ROUND(data!C4,2), " - ", ROUND(data!D4,2),  ")")</f>
+        <v>0.91 (0.73 - 1.13)</v>
+      </c>
+      <c r="G4" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B5, 2), " (", ROUND(data!C5,2), " - ", ROUND(data!D5,2),  ")")</f>
+        <v>1.1 (1.02 - 1.19)</v>
+      </c>
+      <c r="H4" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B6, 2), " (", ROUND(data!C6,2), " - ", ROUND(data!D6,2),  ")")</f>
+        <v>1.16 (1.05 - 1.28)</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="16"/>
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B18, 2), " (", ROUND(data!C18,2), " - ", ROUND(data!D18,2),  ")")</f>
+        <v>1.07 (1.01 - 1.12)</v>
+      </c>
+      <c r="E5" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B19, 2), " (", ROUND(data!C19,2), " - ", ROUND(data!D19,2),  ")")</f>
         <v>1.02 (0.93 - 1.11)</v>
       </c>
-      <c r="F4" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B4, 2), " (", ROUND(MIMIC!C4,2), " - ", ROUND(MIMIC!D4,2),  ")")</f>
-        <v>0.92 (0.74 - 1.14)</v>
-      </c>
-      <c r="G4" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B5, 2), " (", ROUND(MIMIC!C5,2), " - ", ROUND(MIMIC!D5,2),  ")")</f>
-        <v>1.1 (1.02 - 1.19)</v>
-      </c>
-      <c r="H4" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B6, 2), " (", ROUND(MIMIC!C6,2), " - ", ROUND(MIMIC!D6,2),  ")")</f>
-        <v>1.16 (1.05 - 1.28)</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B20, 2), " (", ROUND(data!C20,2), " - ", ROUND(data!D20,2),  ")")</f>
+        <v>0.99 (0.91 - 1.09)</v>
+      </c>
+      <c r="G5" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B21, 2), " (", ROUND(data!C21,2), " - ", ROUND(data!D21,2),  ")")</f>
+        <v>1 (0.85 - 1.18)</v>
+      </c>
+      <c r="H5" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B22, 2), " (", ROUND(data!C22,2), " - ", ROUND(data!D22,2),  ")")</f>
+        <v>1.2 (1.03 - 1.39)</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B7, 2), " (", ROUND(data!C7,2), " - ", ROUND(data!D7,2),  ")")</f>
+        <v>0.85 (0.78 - 0.92)</v>
+      </c>
+      <c r="E6" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B8, 2), " (", ROUND(data!C8,2), " - ", ROUND(data!D8,2),  ")")</f>
+        <v>0.89 (0.69 - 1.17)</v>
+      </c>
+      <c r="F6" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B9, 2), " (", ROUND(data!C9,2), " - ", ROUND(data!D9,2),  ")")</f>
+        <v>1.07 (0.9 - 1.26)</v>
+      </c>
+      <c r="G6" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B10, 2), " (", ROUND(data!C10,2), " - ", ROUND(data!D10,2),  ")")</f>
+        <v>0.78 (0.67 - 0.9)</v>
+      </c>
+      <c r="H6" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B11, 2), " (", ROUND(data!C11,2), " - ", ROUND(data!D11,2),  ")")</f>
+        <v>0.8 (0.7 - 0.91)</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="16"/>
+      <c r="C7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B18, 2), " (", ROUND(MIMIC!C18,2), " - ", ROUND(MIMIC!D18,2),  ")")</f>
-        <v>1.08 (1.02 - 1.13)</v>
-      </c>
-      <c r="E5" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B19, 2), " (", ROUND(MIMIC!C19,2), " - ", ROUND(MIMIC!D19,2),  ")")</f>
-        <v>1.04 (0.95 - 1.13)</v>
-      </c>
-      <c r="F5" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B20, 2), " (", ROUND(MIMIC!C20,2), " - ", ROUND(MIMIC!D20,2),  ")")</f>
-        <v>1 (0.92 - 1.1)</v>
-      </c>
-      <c r="G5" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B21, 2), " (", ROUND(MIMIC!C21,2), " - ", ROUND(MIMIC!D21,2),  ")")</f>
-        <v>1.01 (0.87 - 1.19)</v>
-      </c>
-      <c r="H5" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B22, 2), " (", ROUND(MIMIC!C22,2), " - ", ROUND(MIMIC!D22,2),  ")")</f>
-        <v>1.18 (1.02 - 1.38)</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="D7" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B23, 2), " (", ROUND(data!C23,2), " - ", ROUND(data!D23,2),  ")")</f>
+        <v>0.8 (0.74 - 0.87)</v>
+      </c>
+      <c r="E7" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B24, 2), " (", ROUND(data!C24,2), " - ", ROUND(data!D24,2),  ")")</f>
+        <v>0.68 (0.6 - 0.79)</v>
+      </c>
+      <c r="F7" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B25, 2), " (", ROUND(data!C25,2), " - ", ROUND(data!D25,2),  ")")</f>
+        <v>0.8 (0.69 - 0.92)</v>
+      </c>
+      <c r="G7" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B26, 2), " (", ROUND(data!C26,2), " - ", ROUND(data!D26,2),  ")")</f>
+        <v>0.97 (0.83 - 1.15)</v>
+      </c>
+      <c r="H7" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B27, 2), " (", ROUND(data!C27,2), " - ", ROUND(data!D27,2),  ")")</f>
+        <v>0.9 (0.74 - 1.1)</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B7, 2), " (", ROUND(MIMIC!C7,2), " - ", ROUND(MIMIC!D7,2),  ")")</f>
-        <v>0.84 (0.78 - 0.91)</v>
-      </c>
-      <c r="E6" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B8, 2), " (", ROUND(MIMIC!C8,2), " - ", ROUND(MIMIC!D8,2),  ")")</f>
-        <v>0.88 (0.68 - 1.15)</v>
-      </c>
-      <c r="F6" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B9, 2), " (", ROUND(MIMIC!C9,2), " - ", ROUND(MIMIC!D9,2),  ")")</f>
-        <v>1.07 (0.91 - 1.26)</v>
-      </c>
-      <c r="G6" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B10, 2), " (", ROUND(MIMIC!C10,2), " - ", ROUND(MIMIC!D10,2),  ")")</f>
-        <v>0.77 (0.67 - 0.89)</v>
-      </c>
-      <c r="H6" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B11, 2), " (", ROUND(MIMIC!C11,2), " - ", ROUND(MIMIC!D11,2),  ")")</f>
-        <v>0.79 (0.7 - 0.91)</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="9" t="s">
+      <c r="D8" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B12, 2), " (", ROUND(data!C12,2), " - ", ROUND(data!D12,2),  ")")</f>
+        <v>1.21 (1.15 - 1.27)</v>
+      </c>
+      <c r="E8" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B13, 2), " (", ROUND(data!C13,2), " - ", ROUND(data!D13,2),  ")")</f>
+        <v>1.14 (1.05 - 1.25)</v>
+      </c>
+      <c r="F8" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B14, 2), " (", ROUND(data!C14,2), " - ", ROUND(data!D14,2),  ")")</f>
+        <v>1.12 (0.86 - 1.44)</v>
+      </c>
+      <c r="G8" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B15, 2), " (", ROUND(data!C15,2), " - ", ROUND(data!D15,2),  ")")</f>
+        <v>1.23 (1.15 - 1.33)</v>
+      </c>
+      <c r="H8" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B16, 2), " (", ROUND(data!C16,2), " - ", ROUND(data!D16,2),  ")")</f>
+        <v>1.26 (1.15 - 1.39)</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="16"/>
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B23, 2), " (", ROUND(MIMIC!C23,2), " - ", ROUND(MIMIC!D23,2),  ")")</f>
-        <v>0.8 (0.74 - 0.86)</v>
-      </c>
-      <c r="E7" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B24, 2), " (", ROUND(MIMIC!C24,2), " - ", ROUND(MIMIC!D24,2),  ")")</f>
-        <v>0.68 (0.59 - 0.78)</v>
-      </c>
-      <c r="F7" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B25, 2), " (", ROUND(MIMIC!C25,2), " - ", ROUND(MIMIC!D25,2),  ")")</f>
-        <v>0.79 (0.69 - 0.91)</v>
-      </c>
-      <c r="G7" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B26, 2), " (", ROUND(MIMIC!C26,2), " - ", ROUND(MIMIC!D26,2),  ")")</f>
-        <v>0.97 (0.83 - 1.15)</v>
-      </c>
-      <c r="H7" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B27, 2), " (", ROUND(MIMIC!C27,2), " - ", ROUND(MIMIC!D27,2),  ")")</f>
-        <v>0.91 (0.75 - 1.11)</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B12, 2), " (", ROUND(MIMIC!C12,2), " - ", ROUND(MIMIC!D12,2),  ")")</f>
-        <v>1.21 (1.15 - 1.27)</v>
-      </c>
-      <c r="E8" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B13, 2), " (", ROUND(MIMIC!C13,2), " - ", ROUND(MIMIC!D13,2),  ")")</f>
-        <v>1.14 (1.04 - 1.24)</v>
-      </c>
-      <c r="F8" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B14, 2), " (", ROUND(MIMIC!C14,2), " - ", ROUND(MIMIC!D14,2),  ")")</f>
-        <v>1.12 (0.86 - 1.44)</v>
-      </c>
-      <c r="G8" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B15, 2), " (", ROUND(MIMIC!C15,2), " - ", ROUND(MIMIC!D15,2),  ")")</f>
-        <v>1.24 (1.15 - 1.34)</v>
-      </c>
-      <c r="H8" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B16, 2), " (", ROUND(MIMIC!C16,2), " - ", ROUND(MIMIC!D16,2),  ")")</f>
-        <v>1.27 (1.15 - 1.4)</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="19"/>
-      <c r="C9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B28, 2), " (", ROUND(MIMIC!C28,2), " - ", ROUND(MIMIC!D28,2),  ")")</f>
+      <c r="D9" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B28, 2), " (", ROUND(data!C28,2), " - ", ROUND(data!D28,2),  ")")</f>
         <v>1.14 (1.09 - 1.19)</v>
       </c>
-      <c r="E9" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B29, 2), " (", ROUND(MIMIC!C29,2), " - ", ROUND(MIMIC!D29,2),  ")")</f>
+      <c r="E9" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B29, 2), " (", ROUND(data!C29,2), " - ", ROUND(data!D29,2),  ")")</f>
         <v>1.26 (1.17 - 1.36)</v>
       </c>
-      <c r="F9" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B30, 2), " (", ROUND(MIMIC!C30,2), " - ", ROUND(MIMIC!D30,2),  ")")</f>
+      <c r="F9" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B30, 2), " (", ROUND(data!C30,2), " - ", ROUND(data!D30,2),  ")")</f>
         <v>1.17 (1.07 - 1.27)</v>
       </c>
-      <c r="G9" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B31, 2), " (", ROUND(MIMIC!C31,2), " - ", ROUND(MIMIC!D31,2),  ")")</f>
-        <v>0.93 (0.85 - 1.03)</v>
-      </c>
-      <c r="H9" s="12" t="str">
-        <f>_xlfn.CONCAT(ROUND(MIMIC!B32, 2), " (", ROUND(MIMIC!C32,2), " - ", ROUND(MIMIC!D32,2),  ")")</f>
+      <c r="G9" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B31, 2), " (", ROUND(data!C31,2), " - ", ROUND(data!D31,2),  ")")</f>
+        <v>0.94 (0.85 - 1.03)</v>
+      </c>
+      <c r="H9" s="15" t="str">
+        <f>_xlfn.CONCAT(ROUND(data!B32, 2), " (", ROUND(data!C32,2), " - ", ROUND(data!D32,2),  ")")</f>
         <v>1.01 (0.89 - 1.15)</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit to do pull
</commit_message>
<xml_diff>
--- a/results/Paper/table2_LogReg nice.xlsx
+++ b/results/Paper/table2_LogReg nice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE72E92-F5A3-FF4F-B9D7-98C15C26F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EC2F20-566C-0F4A-AEE7-80A72C826F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="740" windowWidth="19060" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15500" yWindow="760" windowWidth="19060" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -84,29 +84,29 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Odds Ratio (CI)
+    <t>OASIS</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Ranges</t>
+  </si>
+  <si>
+    <t>7 - 10 / 46 - 51</t>
+  </si>
+  <si>
+    <t>0 - 3 / 0 - 37</t>
+  </si>
+  <si>
+    <t>&gt; 10 / &gt; 51</t>
+  </si>
+  <si>
+    <t>4 - 6 / 38 - 45</t>
+  </si>
+  <si>
+    <t>Odds Ratio (95% CI)
  White vs. Non-White</t>
-  </si>
-  <si>
-    <t>OASIS</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Ranges</t>
-  </si>
-  <si>
-    <t>7 - 10 / 46 - 51</t>
-  </si>
-  <si>
-    <t>0 - 3 / 0 - 37</t>
-  </si>
-  <si>
-    <t>&gt; 10 / &gt; 51</t>
-  </si>
-  <si>
-    <t>4 - 6 / 38 - 45</t>
   </si>
 </sst>
 </file>
@@ -204,6 +204,21 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,22 +231,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -554,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
+    <sheetView zoomScale="183" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
@@ -581,21 +581,21 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -899,7 +899,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46007BA-F4A7-5F42-81F4-3F357B170096}">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView zoomScale="196" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1153,199 +1153,199 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="4" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="str">
+      <c r="D4" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B2, 2), " (", ROUND(data!C2,2), " - ", ROUND(data!D2,2),  ")")</f>
         <v>1.08 (1.03 - 1.13)</v>
       </c>
-      <c r="E4" s="15" t="str">
+      <c r="E4" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B3, 2), " (", ROUND(data!C3,2), " - ", ROUND(data!D3,2),  ")")</f>
         <v>1.01 (0.93 - 1.11)</v>
       </c>
-      <c r="F4" s="15" t="str">
+      <c r="F4" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B4, 2), " (", ROUND(data!C4,2), " - ", ROUND(data!D4,2),  ")")</f>
         <v>0.91 (0.73 - 1.13)</v>
       </c>
-      <c r="G4" s="15" t="str">
+      <c r="G4" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B5, 2), " (", ROUND(data!C5,2), " - ", ROUND(data!D5,2),  ")")</f>
         <v>1.1 (1.02 - 1.19)</v>
       </c>
-      <c r="H4" s="15" t="str">
+      <c r="H4" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B6, 2), " (", ROUND(data!C6,2), " - ", ROUND(data!D6,2),  ")")</f>
         <v>1.16 (1.05 - 1.28)</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="16"/>
-      <c r="C5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="15" t="str">
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B18, 2), " (", ROUND(data!C18,2), " - ", ROUND(data!D18,2),  ")")</f>
         <v>1.07 (1.01 - 1.12)</v>
       </c>
-      <c r="E5" s="15" t="str">
+      <c r="E5" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B19, 2), " (", ROUND(data!C19,2), " - ", ROUND(data!D19,2),  ")")</f>
         <v>1.02 (0.93 - 1.11)</v>
       </c>
-      <c r="F5" s="15" t="str">
+      <c r="F5" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B20, 2), " (", ROUND(data!C20,2), " - ", ROUND(data!D20,2),  ")")</f>
         <v>0.99 (0.91 - 1.09)</v>
       </c>
-      <c r="G5" s="15" t="str">
+      <c r="G5" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B21, 2), " (", ROUND(data!C21,2), " - ", ROUND(data!D21,2),  ")")</f>
         <v>1 (0.85 - 1.18)</v>
       </c>
-      <c r="H5" s="15" t="str">
+      <c r="H5" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B22, 2), " (", ROUND(data!C22,2), " - ", ROUND(data!D22,2),  ")")</f>
         <v>1.2 (1.03 - 1.39)</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="15" t="str">
+      <c r="D6" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B7, 2), " (", ROUND(data!C7,2), " - ", ROUND(data!D7,2),  ")")</f>
         <v>0.85 (0.78 - 0.92)</v>
       </c>
-      <c r="E6" s="15" t="str">
+      <c r="E6" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B8, 2), " (", ROUND(data!C8,2), " - ", ROUND(data!D8,2),  ")")</f>
         <v>0.89 (0.69 - 1.17)</v>
       </c>
-      <c r="F6" s="15" t="str">
+      <c r="F6" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B9, 2), " (", ROUND(data!C9,2), " - ", ROUND(data!D9,2),  ")")</f>
         <v>1.07 (0.9 - 1.26)</v>
       </c>
-      <c r="G6" s="15" t="str">
+      <c r="G6" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B10, 2), " (", ROUND(data!C10,2), " - ", ROUND(data!D10,2),  ")")</f>
         <v>0.78 (0.67 - 0.9)</v>
       </c>
-      <c r="H6" s="15" t="str">
+      <c r="H6" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B11, 2), " (", ROUND(data!C11,2), " - ", ROUND(data!D11,2),  ")")</f>
         <v>0.8 (0.7 - 0.91)</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="16"/>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="15" t="str">
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B23, 2), " (", ROUND(data!C23,2), " - ", ROUND(data!D23,2),  ")")</f>
         <v>0.8 (0.74 - 0.87)</v>
       </c>
-      <c r="E7" s="15" t="str">
+      <c r="E7" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B24, 2), " (", ROUND(data!C24,2), " - ", ROUND(data!D24,2),  ")")</f>
         <v>0.68 (0.6 - 0.79)</v>
       </c>
-      <c r="F7" s="15" t="str">
+      <c r="F7" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B25, 2), " (", ROUND(data!C25,2), " - ", ROUND(data!D25,2),  ")")</f>
         <v>0.8 (0.69 - 0.92)</v>
       </c>
-      <c r="G7" s="15" t="str">
+      <c r="G7" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B26, 2), " (", ROUND(data!C26,2), " - ", ROUND(data!D26,2),  ")")</f>
         <v>0.97 (0.83 - 1.15)</v>
       </c>
-      <c r="H7" s="15" t="str">
+      <c r="H7" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B27, 2), " (", ROUND(data!C27,2), " - ", ROUND(data!D27,2),  ")")</f>
         <v>0.9 (0.74 - 1.1)</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="15" t="str">
+      <c r="D8" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B12, 2), " (", ROUND(data!C12,2), " - ", ROUND(data!D12,2),  ")")</f>
         <v>1.21 (1.15 - 1.27)</v>
       </c>
-      <c r="E8" s="15" t="str">
+      <c r="E8" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B13, 2), " (", ROUND(data!C13,2), " - ", ROUND(data!D13,2),  ")")</f>
         <v>1.14 (1.05 - 1.25)</v>
       </c>
-      <c r="F8" s="15" t="str">
+      <c r="F8" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B14, 2), " (", ROUND(data!C14,2), " - ", ROUND(data!D14,2),  ")")</f>
         <v>1.12 (0.86 - 1.44)</v>
       </c>
-      <c r="G8" s="15" t="str">
+      <c r="G8" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B15, 2), " (", ROUND(data!C15,2), " - ", ROUND(data!D15,2),  ")")</f>
         <v>1.23 (1.15 - 1.33)</v>
       </c>
-      <c r="H8" s="15" t="str">
+      <c r="H8" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B16, 2), " (", ROUND(data!C16,2), " - ", ROUND(data!D16,2),  ")")</f>
         <v>1.26 (1.15 - 1.39)</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="16"/>
-      <c r="C9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="15" t="str">
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B28, 2), " (", ROUND(data!C28,2), " - ", ROUND(data!D28,2),  ")")</f>
         <v>1.14 (1.09 - 1.19)</v>
       </c>
-      <c r="E9" s="15" t="str">
+      <c r="E9" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B29, 2), " (", ROUND(data!C29,2), " - ", ROUND(data!D29,2),  ")")</f>
         <v>1.26 (1.17 - 1.36)</v>
       </c>
-      <c r="F9" s="15" t="str">
+      <c r="F9" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B30, 2), " (", ROUND(data!C30,2), " - ", ROUND(data!D30,2),  ")")</f>
         <v>1.17 (1.07 - 1.27)</v>
       </c>
-      <c r="G9" s="15" t="str">
+      <c r="G9" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B31, 2), " (", ROUND(data!C31,2), " - ", ROUND(data!D31,2),  ")")</f>
         <v>0.94 (0.85 - 1.03)</v>
       </c>
-      <c r="H9" s="15" t="str">
+      <c r="H9" s="10" t="str">
         <f>_xlfn.CONCAT(ROUND(data!B32, 2), " (", ROUND(data!C32,2), " - ", ROUND(data!D32,2),  ")")</f>
         <v>1.01 (0.89 - 1.15)</v>
       </c>

</xml_diff>